<commit_message>
Update PM10 tidsregistrering for Nikolaj
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Dokumenter/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="8_{96A3C360-5D43-4E60-8FD6-C6F4EBA01892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{9B85F74B-ACAA-4C5C-ACE3-EEBB9AE51DA5}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="8_{96A3C360-5D43-4E60-8FD6-C6F4EBA01892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{59F07086-4D9D-4635-86CA-42076F52CF80}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
   <si>
     <t>Dato</t>
   </si>
@@ -181,6 +181,27 @@
   </si>
   <si>
     <t>30 min</t>
+  </si>
+  <si>
+    <t>Operations kontrakt OC0801</t>
+  </si>
+  <si>
+    <t>Kravworkshop</t>
+  </si>
+  <si>
+    <t>1:30 timer</t>
+  </si>
+  <si>
+    <t>2 timer og 30 min</t>
+  </si>
+  <si>
+    <t>Usecase 07 indtjeningsbidrag</t>
+  </si>
+  <si>
+    <t>Domæne model 07</t>
+  </si>
+  <si>
+    <t>Networking (Virksomhedsdag datamatiker)</t>
   </si>
 </sst>
 </file>
@@ -331,7 +352,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -377,6 +398,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -757,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:H48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -979,87 +1003,163 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C9" s="13"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="18"/>
+      <c r="A9" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D9" s="14">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E9" s="14">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="G9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H9" s="1">
         <f>SUM(G$3:G9)</f>
-        <v>0.49652777777777768</v>
+        <v>0.51736111111111105</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C10" s="13"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="18"/>
+      <c r="A10" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D10" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="E10" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>51</v>
+      </c>
       <c r="G10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H10" s="1">
         <f>SUM(G$3:G10)</f>
-        <v>0.49652777777777768</v>
+        <v>0.57986111111111105</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C11" s="13"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="18"/>
+      <c r="A11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H11" s="1">
         <f>SUM(G$3:G11)</f>
-        <v>0.49652777777777768</v>
+        <v>0.62152777777777768</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="18"/>
+      <c r="A12" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D12" s="14">
+        <v>0.5625</v>
+      </c>
+      <c r="E12" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="G12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="H12" s="1">
         <f>SUM(G$3:G12)</f>
-        <v>0.49652777777777768</v>
+        <v>0.64236111111111105</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C13" s="13"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="18"/>
+      <c r="A13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D13" s="14">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E13" s="14">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>48</v>
+      </c>
       <c r="G13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0833333333333259E-2</v>
       </c>
       <c r="H13" s="1">
         <f>SUM(G$3:G13)</f>
-        <v>0.49652777777777768</v>
+        <v>0.66319444444444431</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C14" s="13"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
+      <c r="A14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="13">
+        <v>43887</v>
+      </c>
+      <c r="D14" s="14">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E14" s="14">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="F14" s="18"/>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="H14" s="1">
         <f>SUM(G$3:G14)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1071,7 +1171,7 @@
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1083,7 +1183,7 @@
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1095,7 +1195,7 @@
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1107,7 +1207,7 @@
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1119,7 +1219,7 @@
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1131,7 +1231,7 @@
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1143,7 +1243,7 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1155,7 +1255,7 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1167,7 +1267,7 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1179,7 +1279,7 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1191,7 +1291,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1202,7 +1302,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1213,7 +1313,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1224,7 +1324,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1235,7 +1335,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1246,7 +1346,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1257,7 +1357,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1268,7 +1368,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1279,7 +1379,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>0.49652777777777768</v>
+        <v>0.70486111111111105</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update tidsregistrering for Nikolaj
Update tidsregistrering for Nikolaj
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Dokumenter/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Skrivebord/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="90" documentId="8_{96A3C360-5D43-4E60-8FD6-C6F4EBA01892}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{59F07086-4D9D-4635-86CA-42076F52CF80}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{996E4986-AD92-451D-BB40-35758B227468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Roller">'Ark2'!$B$3:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
   <si>
     <t>Dato</t>
   </si>
@@ -202,6 +205,24 @@
   </si>
   <si>
     <t>Networking (Virksomhedsdag datamatiker)</t>
+  </si>
+  <si>
+    <t>SD 0802</t>
+  </si>
+  <si>
+    <t>DCD 0802</t>
+  </si>
+  <si>
+    <t>UnitTests 0102</t>
+  </si>
+  <si>
+    <t>2½ time</t>
+  </si>
+  <si>
+    <t>Operations kontrakt OC0803</t>
+  </si>
+  <si>
+    <t>DCD OG SD 0802 (rettet)</t>
   </si>
 </sst>
 </file>
@@ -352,7 +373,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="6" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -393,14 +414,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -779,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -796,19 +821,19 @@
     <col min="8" max="8" width="37.21875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:9" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A1" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-    </row>
-    <row r="2" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A2" s="7" t="s">
         <v>36</v>
       </c>
@@ -834,7 +859,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>40</v>
       </c>
@@ -861,8 +886,9 @@
         <f>SUM(G$3:G3)</f>
         <v>0.26388888888888895</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="I3" s="22"/>
+    </row>
+    <row r="4" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
         <v>42</v>
       </c>
@@ -890,7 +916,7 @@
         <v>0.29166666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>42</v>
       </c>
@@ -918,7 +944,7 @@
         <v>0.37152777777777768</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>45</v>
       </c>
@@ -946,7 +972,7 @@
         <v>0.38888888888888878</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
         <v>45</v>
       </c>
@@ -974,7 +1000,7 @@
         <v>0.4097222222222221</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A8" s="11" t="s">
         <v>46</v>
       </c>
@@ -1002,7 +1028,7 @@
         <v>0.49652777777777768</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A9" s="11" t="s">
         <v>49</v>
       </c>
@@ -1030,7 +1056,7 @@
         <v>0.51736111111111105</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>50</v>
       </c>
@@ -1058,7 +1084,7 @@
         <v>0.57986111111111105</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A11" s="11" t="s">
         <v>50</v>
       </c>
@@ -1074,7 +1100,7 @@
       <c r="E11" s="14">
         <v>0.5625</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="20" t="s">
         <v>52</v>
       </c>
       <c r="G11" s="5">
@@ -1086,7 +1112,7 @@
         <v>0.62152777777777768</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
         <v>53</v>
       </c>
@@ -1114,7 +1140,7 @@
         <v>0.64236111111111105</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A13" s="11" t="s">
         <v>54</v>
       </c>
@@ -1139,7 +1165,7 @@
         <v>0.66319444444444431</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
       <c r="A14" s="11" t="s">
         <v>55</v>
       </c>
@@ -1152,7 +1178,9 @@
       <c r="E14" s="14">
         <v>0.64583333333333337</v>
       </c>
-      <c r="F14" s="18"/>
+      <c r="F14" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>4.1666666666666741E-2</v>
@@ -1162,79 +1190,167 @@
         <v>0.70486111111111105</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C15" s="13"/>
-      <c r="F15" s="18"/>
+    <row r="15" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A15" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="13">
+        <v>43892</v>
+      </c>
+      <c r="D15" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E15" s="15">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>43</v>
+      </c>
       <c r="G15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.10416666666666669</v>
       </c>
       <c r="H15" s="1">
         <f>SUM(G$3:G15)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C16" s="13"/>
+        <v>0.80902777777777768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="13">
+        <v>43892</v>
+      </c>
+      <c r="D16" s="15">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E16" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F16" s="18"/>
       <c r="G16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.555555555555558E-2</v>
       </c>
       <c r="H16" s="1">
         <f>SUM(G$3:G16)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C17" s="13"/>
-      <c r="F17" s="18"/>
+        <v>0.86458333333333326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A17" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="13">
+        <v>43892</v>
+      </c>
+      <c r="D17" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E17" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>59</v>
+      </c>
       <c r="G17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H17" s="1">
         <f>SUM(G$3:G17)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C18" s="13"/>
-      <c r="F18" s="18"/>
+        <v>0.90624999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A18" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="13">
+        <v>43893</v>
+      </c>
+      <c r="D18" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E18" s="15">
+        <v>0.4236111111111111</v>
+      </c>
+      <c r="F18" s="21"/>
       <c r="G18" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.8611111111111105E-2</v>
       </c>
       <c r="H18" s="1">
         <f>SUM(G$3:G18)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C19" s="13"/>
+        <v>0.95486111111111094</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A19" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="13">
+        <v>43893</v>
+      </c>
+      <c r="D19" s="15">
+        <v>0.52777777777777779</v>
+      </c>
+      <c r="E19" s="15">
+        <v>0.59722222222222221</v>
+      </c>
       <c r="F19" s="18"/>
       <c r="G19" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.944444444444442E-2</v>
       </c>
       <c r="H19" s="1">
         <f>SUM(G$3:G19)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C20" s="13"/>
+        <v>1.0243055555555554</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A20" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="13">
+        <v>43893</v>
+      </c>
+      <c r="D20" s="15">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E20" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F20" s="18"/>
       <c r="G20" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H20" s="1">
         <f>SUM(G$3:G20)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C21" s="13"/>
       <c r="F21" s="18"/>
       <c r="G21" s="5">
@@ -1243,10 +1359,10 @@
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C22" s="13"/>
       <c r="F22" s="18"/>
       <c r="G22" s="5">
@@ -1255,10 +1371,10 @@
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C23" s="13"/>
       <c r="F23" s="18"/>
       <c r="G23" s="5">
@@ -1267,10 +1383,10 @@
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C24" s="13"/>
       <c r="F24" s="18"/>
       <c r="G24" s="5">
@@ -1279,10 +1395,10 @@
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C25" s="13"/>
       <c r="F25" s="18"/>
       <c r="G25" s="5">
@@ -1291,10 +1407,10 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C26" s="13"/>
       <c r="G26" s="5">
         <f t="shared" si="0"/>
@@ -1302,10 +1418,10 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C27" s="13"/>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
@@ -1313,10 +1429,10 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="28" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C28" s="13"/>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
@@ -1324,10 +1440,10 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C29" s="13"/>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
@@ -1335,10 +1451,10 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="30" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C30" s="13"/>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
@@ -1346,10 +1462,10 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C31" s="13"/>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
@@ -1357,10 +1473,10 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>0.70486111111111105</v>
-      </c>
-    </row>
-    <row r="32" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
+        <v>1.0868055555555554</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
       <c r="C32" s="13"/>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
@@ -1368,7 +1484,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>0.70486111111111105</v>
+        <v>1.0868055555555554</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1379,7 +1495,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>0.70486111111111105</v>
+        <v>1.0868055555555554</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">
@@ -1464,13 +1580,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
Update Tidsregistrering for PM10 - Nikolaj
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffadfded41a68b1b/Skrivebord/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{996E4986-AD92-451D-BB40-35758B227468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{996E4986-AD92-451D-BB40-35758B227468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E118527E-BFE0-40FB-B7F5-727EC117D7AF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="Roller">'Ark2'!$B$3:$B$31</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
   <si>
     <t>Dato</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>DCD OG SD 0802 (rettet)</t>
+  </si>
+  <si>
+    <t>ATD 11</t>
+  </si>
+  <si>
+    <t>DD 11</t>
+  </si>
+  <si>
+    <t>AD 11</t>
   </si>
 </sst>
 </file>
@@ -806,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1351,51 +1360,107 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C21" s="13"/>
+      <c r="A21" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="13">
+        <v>43894</v>
+      </c>
+      <c r="D21" s="15">
+        <v>0.59375</v>
+      </c>
+      <c r="E21" s="15">
+        <v>0.625</v>
+      </c>
       <c r="F21" s="18"/>
       <c r="G21" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.125E-2</v>
       </c>
       <c r="H21" s="1">
         <f>SUM(G$3:G21)</f>
-        <v>1.0868055555555554</v>
+        <v>1.1180555555555554</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C22" s="13"/>
+      <c r="A22" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="13">
+        <v>43894</v>
+      </c>
+      <c r="D22" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="E22" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F22" s="18"/>
       <c r="G22" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H22" s="1">
         <f>SUM(G$3:G22)</f>
-        <v>1.0868055555555554</v>
+        <v>1.1597222222222219</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C23" s="13"/>
+      <c r="A23" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="13">
+        <v>43894</v>
+      </c>
+      <c r="D23" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="E23" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F23" s="18"/>
       <c r="G23" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H23" s="1">
         <f>SUM(G$3:G23)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2013888888888884</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C24" s="13"/>
+      <c r="A24" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="13">
+        <v>43894</v>
+      </c>
+      <c r="D24" s="15">
+        <v>0.625</v>
+      </c>
+      <c r="E24" s="15">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="F24" s="18"/>
       <c r="G24" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H24" s="1">
         <f>SUM(G$3:G24)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1407,7 +1472,7 @@
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1418,7 +1483,7 @@
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1429,7 +1494,7 @@
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1440,7 +1505,7 @@
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1451,7 +1516,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1462,7 +1527,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1473,7 +1538,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1484,7 +1549,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1495,7 +1560,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>1.0868055555555554</v>
+        <v>1.2430555555555549</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Tidsregis pm 10 Nikolaj
Coauthor : Ingen
Reveiwer : Ingen
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{996E4986-AD92-451D-BB40-35758B227468}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E118527E-BFE0-40FB-B7F5-727EC117D7AF}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="114_{D9A70605-BEF5-46E8-8909-F6049821E82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E667AFD-FC9F-4F84-9B45-312C647DE9D3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
   <si>
     <t>Dato</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>AD 11</t>
+  </si>
+  <si>
+    <t>DD OG AD 10(11) forsat</t>
+  </si>
+  <si>
+    <t>ATD 10</t>
+  </si>
+  <si>
+    <t>DCD0803</t>
+  </si>
+  <si>
+    <t>SD 0803</t>
   </si>
 </sst>
 </file>
@@ -815,8 +827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B11" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,48 +1476,104 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C25" s="13"/>
+      <c r="A25" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="13">
+        <v>43895</v>
+      </c>
+      <c r="D25" s="15">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E25" s="15">
+        <v>0.41666666666666669</v>
+      </c>
       <c r="F25" s="18"/>
       <c r="G25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H25" s="1">
         <f>SUM(G$3:G25)</f>
-        <v>1.2430555555555549</v>
+        <v>1.3055555555555549</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C26" s="13"/>
+      <c r="A26" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="13">
+        <v>43895</v>
+      </c>
+      <c r="D26" s="15">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="E26" s="15">
+        <v>0.47916666666666669</v>
+      </c>
       <c r="G26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H26" s="1">
         <f>SUM(G$3:G26)</f>
-        <v>1.2430555555555549</v>
+        <v>1.3680555555555549</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C27" s="13"/>
+      <c r="A27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="13">
+        <v>43895</v>
+      </c>
+      <c r="D27" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E27" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G27" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H27" s="1">
         <f>SUM(G$3:G27)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4305555555555549</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C28" s="13"/>
+      <c r="A28" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="13">
+        <v>43895</v>
+      </c>
+      <c r="D28" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E28" s="15">
+        <v>0.65277777777777779</v>
+      </c>
       <c r="G28" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.944444444444442E-2</v>
       </c>
       <c r="H28" s="1">
         <f>SUM(G$3:G28)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1516,7 +1584,7 @@
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1527,7 +1595,7 @@
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1538,7 +1606,7 @@
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1549,7 +1617,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1560,7 +1628,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>1.2430555555555549</v>
+        <v>1.4999999999999993</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update for Tidsregistrering PM10 Nikolaj
CoAuthor: ingen
Reviewer : ingen
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="114_{D9A70605-BEF5-46E8-8909-F6049821E82C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4E667AFD-FC9F-4F84-9B45-312C647DE9D3}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="114_{1FBD5424-5E74-4268-A172-239ABCE5DA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{402A0B74-A8BF-4131-A935-C75A9891EEB2}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
   <si>
     <t>Dato</t>
   </si>
@@ -244,6 +244,15 @@
   </si>
   <si>
     <t>SD 0803</t>
+  </si>
+  <si>
+    <t>Lavet implement af OC0803</t>
+  </si>
+  <si>
+    <t>implenter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavet UI UC04 </t>
   </si>
 </sst>
 </file>
@@ -827,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1577,36 +1586,78 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C29" s="13"/>
+      <c r="A29" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="13">
+        <v>43896</v>
+      </c>
+      <c r="D29" s="15">
+        <v>0.375</v>
+      </c>
+      <c r="E29" s="15">
+        <v>0.47222222222222227</v>
+      </c>
       <c r="G29" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.7222222222222265E-2</v>
       </c>
       <c r="H29" s="1">
         <f>SUM(G$3:G29)</f>
-        <v>1.4999999999999993</v>
+        <v>1.5972222222222217</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C30" s="13"/>
+      <c r="A30" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="13">
+        <v>43896</v>
+      </c>
+      <c r="D30" s="15">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E30" s="15">
+        <v>0.5625</v>
+      </c>
       <c r="G30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="H30" s="1">
         <f>SUM(G$3:G30)</f>
-        <v>1.4999999999999993</v>
+        <v>1.6388888888888884</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C31" s="13"/>
+      <c r="A31" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="13">
+        <v>43896</v>
+      </c>
+      <c r="D31" s="15">
+        <v>0.5625</v>
+      </c>
+      <c r="E31" s="15">
+        <v>0.61458333333333337</v>
+      </c>
       <c r="G31" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="H31" s="1">
         <f>SUM(G$3:G31)</f>
-        <v>1.4999999999999993</v>
+        <v>1.6909722222222219</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1617,7 +1668,7 @@
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>1.4999999999999993</v>
+        <v>1.6909722222222219</v>
       </c>
     </row>
     <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
@@ -1628,7 +1679,7 @@
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>1.4999999999999993</v>
+        <v>1.6909722222222219</v>
       </c>
     </row>
     <row r="34" spans="3:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Tidsregistrering PM 10 Nikolaj
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="114_{1FBD5424-5E74-4268-A172-239ABCE5DA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{402A0B74-A8BF-4131-A935-C75A9891EEB2}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="114_{1FBD5424-5E74-4268-A172-239ABCE5DA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0299286D-79AE-4C5C-8355-76CB48DF47AE}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
   <si>
     <t>Dato</t>
   </si>
@@ -836,8 +836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1625,6 +1625,9 @@
       </c>
       <c r="E30" s="15">
         <v>0.5625</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>43</v>
       </c>
       <c r="G30" s="5">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Update PM10 Tidsregistreing Nikolaj
</commit_message>
<xml_diff>
--- a/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
+++ b/08 Project Management/Tidsregistrering/PM10 Tidsregistrering for Nikolaj.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikol\OneDrive\Dokumenter\GitHub\HoeKulator\08 Project Management\Tidsregistrering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="114_{1FBD5424-5E74-4268-A172-239ABCE5DA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0299286D-79AE-4C5C-8355-76CB48DF47AE}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="114_{1FBD5424-5E74-4268-A172-239ABCE5DA48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B42568C5-51DC-49A6-A74A-6FA67046D772}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84363544-26A8-43A0-AC4F-33AAA0FF1AA4}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
   <si>
     <t>Dato</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t xml:space="preserve">Lavet UI UC04 </t>
+  </si>
+  <si>
+    <t>SD0701/2/3 og DCD07</t>
+  </si>
+  <si>
+    <t>UC07 implement af OC07</t>
   </si>
 </sst>
 </file>
@@ -836,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A07EC185-8A27-41F3-967D-179793E73F80}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C16" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="119" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1664,70 +1670,98 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C32" s="13"/>
+      <c r="A32" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32" s="13">
+        <v>43901</v>
+      </c>
+      <c r="D32" s="15">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E32" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G32" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.18750000000000006</v>
       </c>
       <c r="H32" s="1">
         <f>SUM(G$3:G32)</f>
-        <v>1.6909722222222219</v>
-      </c>
-    </row>
-    <row r="33" spans="3:8" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="C33" s="13"/>
+        <v>1.8784722222222219</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A33" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="13">
+        <v>43901</v>
+      </c>
+      <c r="D33" s="15">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E33" s="15">
+        <v>0.64583333333333337</v>
+      </c>
       <c r="G33" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H33" s="1">
         <f>SUM(G$3:G33)</f>
-        <v>1.6909722222222219</v>
-      </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.3">
+        <v>1.9409722222222219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C34" s="13"/>
     </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C35" s="13"/>
     </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C36" s="13"/>
     </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C37" s="13"/>
     </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C38" s="13"/>
     </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C39" s="13"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C40" s="13"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C41" s="13"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C42" s="13"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C43" s="13"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C44" s="13"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C45" s="13"/>
     </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C46" s="13"/>
     </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C47" s="13"/>
     </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C48" s="13"/>
     </row>
   </sheetData>

</xml_diff>